<commit_message>
Copied individual files of ORCA Sigma profiles as they might be easier for Jules to understand
</commit_message>
<xml_diff>
--- a/Model_Results_Tabulation.xlsx
+++ b/Model_Results_Tabulation.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/kaslam_uoguelph_ca/Documents/My Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="8_{F5D792F4-EF2B-4940-B29F-D60A5D3F67D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C06CE3AD-5EA4-4B42-A74B-320D099F8B35}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{A0BE6DE1-3CF5-41D0-B09A-BEF2AC4E9CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E20E0EC-A386-4807-8363-59B7A9226132}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{4252826C-2590-47B3-A475-714FD785B948}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4252826C-2590-47B3-A475-714FD785B948}"/>
   </bookViews>
   <sheets>
     <sheet name="Chembl 12C" sheetId="1" r:id="rId1"/>
     <sheet name="IUPAC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>Test MAE</t>
   </si>
@@ -194,6 +193,12 @@
   </si>
   <si>
     <t>8 rdkit molecular features + Gasteiger Charge + Mcginn Sigma Profiles IUPAC</t>
+  </si>
+  <si>
+    <t>Features_Chembl-12C_Mcginn-Sigma-Profile_MLP</t>
+  </si>
+  <si>
+    <t>Chembl 12C Sigma Profiles Mcginn</t>
   </si>
 </sst>
 </file>
@@ -232,7 +237,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,20 +593,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1809039-F9A0-43BD-9B94-739FF8D03AF4}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="95.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84" customWidth="1"/>
+    <col min="2" max="2" width="45.21875" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
     <col min="16" max="16" width="22.109375" customWidth="1"/>
-    <col min="18" max="18" width="3.21875" customWidth="1"/>
+    <col min="18" max="18" width="21.33203125" customWidth="1"/>
     <col min="19" max="19" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -723,35 +728,35 @@
         <v>0.73680000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.61370000000000002</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.44629999999999997</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>0.65380000000000005</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>0.36230000000000001</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>0.8085</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>0.60189999999999999</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>0.56899999999999995</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="3">
         <v>0.74709999999999999</v>
       </c>
     </row>
@@ -959,36 +964,54 @@
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="3">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="D11" s="3">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="F11" s="3">
-        <v>7.8E-2</v>
-      </c>
-      <c r="G11" s="3">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.48</v>
-      </c>
-      <c r="J11" s="3">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="L11" s="3">
-        <v>0.871</v>
-      </c>
-      <c r="M11" s="3">
-        <v>0.99399999999999999</v>
+      <c r="C11" s="2">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="J11" s="2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.996</v>
+      </c>
+      <c r="O11" s="2">
+        <v>3.0219999999999998</v>
+      </c>
+      <c r="P11" s="2">
+        <v>58.148000000000003</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>29.533000000000001</v>
+      </c>
+      <c r="R11" s="2">
+        <v>28.614999999999998</v>
+      </c>
+      <c r="S11" s="2">
+        <v>78.805999999999997</v>
+      </c>
+      <c r="T11" s="2">
+        <v>39.173999999999999</v>
+      </c>
+      <c r="U11" s="2">
+        <v>39.633000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1022,46 +1045,79 @@
       <c r="M12" s="2">
         <v>0.98899999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="O12" s="2">
+        <v>3.891</v>
+      </c>
+      <c r="P12" s="2">
+        <v>57.765999999999998</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>26.931999999999999</v>
+      </c>
+      <c r="R12" s="2">
+        <v>30.834</v>
+      </c>
+      <c r="S12" s="2">
+        <v>79.188999999999993</v>
+      </c>
+      <c r="T12" s="2">
+        <v>35.96</v>
+      </c>
+      <c r="U12" s="2">
+        <v>43.228999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C13">
-        <v>0.72699999999999998</v>
-      </c>
-      <c r="F13">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="I13">
-        <v>1.077</v>
-      </c>
-      <c r="L13">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="O13">
-        <v>8.56</v>
-      </c>
-      <c r="P13">
-        <v>20.966000000000001</v>
-      </c>
-      <c r="Q13">
-        <v>9.6639999999999997</v>
-      </c>
-      <c r="R13">
-        <v>11.303000000000001</v>
-      </c>
-      <c r="S13">
-        <v>39.603000000000002</v>
-      </c>
-      <c r="T13">
-        <v>16.997</v>
-      </c>
-      <c r="U13">
-        <v>22.606000000000002</v>
+      <c r="C13" s="2">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.147</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.258</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1.071</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1.1220000000000001</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="O13" s="2">
+        <v>5.9320000000000004</v>
+      </c>
+      <c r="P13" s="2">
+        <v>17.687999999999999</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>8.7140000000000004</v>
+      </c>
+      <c r="R13" s="2">
+        <v>8.9730000000000008</v>
+      </c>
+      <c r="S13" s="2">
+        <v>33.563000000000002</v>
+      </c>
+      <c r="T13" s="2">
+        <v>15.789</v>
+      </c>
+      <c r="U13" s="2">
+        <v>17.774000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1072,37 +1128,49 @@
         <v>45</v>
       </c>
       <c r="C14" s="2">
-        <v>0.437</v>
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.53800000000000003</v>
       </c>
       <c r="F14" s="2">
-        <v>0.38900000000000001</v>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.65800000000000003</v>
       </c>
       <c r="I14" s="2">
-        <v>0.624</v>
+        <v>0.755</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.81100000000000005</v>
       </c>
       <c r="L14" s="2">
-        <v>0.79100000000000004</v>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.65200000000000002</v>
       </c>
       <c r="O14" s="2">
-        <v>4.9130000000000003</v>
+        <v>5.0410000000000004</v>
       </c>
       <c r="P14" s="2">
-        <v>34.426000000000002</v>
+        <v>30.802</v>
       </c>
       <c r="Q14" s="2">
-        <v>18.981999999999999</v>
+        <v>15.444000000000001</v>
       </c>
       <c r="R14" s="2">
-        <v>15.444000000000001</v>
+        <v>15.358000000000001</v>
       </c>
       <c r="S14" s="2">
-        <v>58.670999999999999</v>
+        <v>51.854999999999997</v>
       </c>
       <c r="T14" s="2">
-        <v>34.426000000000002</v>
+        <v>25.797999999999998</v>
       </c>
       <c r="U14" s="2">
-        <v>24.245000000000001</v>
+        <v>26.056999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1156,6 +1224,59 @@
       </c>
       <c r="U15" s="2">
         <v>37.489199999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.46579999999999999</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.18690000000000001</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.49809999999999999</v>
+      </c>
+      <c r="G16" s="3">
+        <v>6.2700000000000006E-2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.70569999999999999</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.25030000000000002</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0.75229999999999997</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0.9667</v>
+      </c>
+      <c r="O16" s="3">
+        <v>4.4420000000000002</v>
+      </c>
+      <c r="P16" s="3">
+        <v>37.79</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>17.28</v>
+      </c>
+      <c r="R16" s="3">
+        <v>20.51</v>
+      </c>
+      <c r="S16" s="3">
+        <v>60.68</v>
+      </c>
+      <c r="T16" s="3">
+        <v>28.26</v>
+      </c>
+      <c r="U16" s="3">
+        <v>32.43</v>
       </c>
     </row>
   </sheetData>
@@ -1170,7 +1291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E397748-C831-472A-B237-20EADB4566E9}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>